<commit_message>
Fix export to Simapro.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-distribution.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-distribution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E57FA49-D23C-694E-8DCF-8D60EA2073A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490D0725-2A1B-1F40-A9D3-BAB7C04B4AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="27820" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$269</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateCount="10" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -208,12 +208,6 @@
     <t>sheet rolling, chromium steel</t>
   </si>
   <si>
-    <t>Carbon fiber, weaved, at factory</t>
-  </si>
-  <si>
-    <t>Carbon fiber, weaved</t>
-  </si>
-  <si>
     <t>market for epoxy resin, liquid</t>
   </si>
   <si>
@@ -607,6 +601,12 @@
   </si>
   <si>
     <t>transport, freight, lorry, unspecified</t>
+  </si>
+  <si>
+    <t>carbon fiber, weaved</t>
+  </si>
+  <si>
+    <t>carbon fiber production, weaved, at factory</t>
   </si>
 </sst>
 </file>
@@ -666,24 +666,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -972,36 +964,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I269"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="44.5" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -1009,7 +1001,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -1017,15 +1009,15 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -1033,7 +1025,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1041,7 +1033,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1049,7 +1041,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
@@ -1057,12 +1049,12 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
@@ -1091,8 +1083,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>186</v>
+      <c r="A13" t="s">
+        <v>184</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1110,7 +1102,7 @@
         <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1155,7 +1147,7 @@
       <c r="G15" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1178,7 +1170,7 @@
       <c r="G16" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1201,7 +1193,7 @@
       <c r="G17" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1381,7 +1373,7 @@
         <v>47</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G25" t="s">
         <v>23</v>
@@ -1415,8 +1407,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>134</v>
+      <c r="A27" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="B27">
         <v>250</v>
@@ -1433,20 +1425,20 @@
       <c r="G27" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>134</v>
+      <c r="I27" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="A30" t="s">
         <v>1</v>
       </c>
       <c r="B30" t="s">
@@ -1454,7 +1446,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="A31" t="s">
         <v>3</v>
       </c>
       <c r="B31">
@@ -1462,15 +1454,15 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" t="s">
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33" t="s">
@@ -1478,7 +1470,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="A34" t="s">
         <v>7</v>
       </c>
       <c r="B34" t="s">
@@ -1486,7 +1478,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="A35" t="s">
         <v>8</v>
       </c>
       <c r="B35" t="s">
@@ -1494,7 +1486,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+      <c r="A36" t="s">
         <v>10</v>
       </c>
       <c r="B36" t="s">
@@ -1502,12 +1494,12 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
+      <c r="A38" t="s">
         <v>13</v>
       </c>
       <c r="B38" t="s">
@@ -1536,8 +1528,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>134</v>
+      <c r="A39" t="s">
+        <v>132</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -1555,7 +1547,7 @@
         <v>19</v>
       </c>
       <c r="I39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1646,107 +1638,107 @@
       <c r="G43" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="I43" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="5">
+      <c r="A44" t="s">
+        <v>188</v>
+      </c>
+      <c r="B44">
         <v>7.1400000000000006</v>
       </c>
       <c r="C44" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E44" s="5" t="s">
+      <c r="D44" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" t="s">
         <v>22</v>
       </c>
       <c r="G44" t="s">
         <v>23</v>
       </c>
-      <c r="I44" s="5" t="s">
-        <v>57</v>
+      <c r="I44" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="5">
+        <v>56</v>
+      </c>
+      <c r="B45">
         <v>3.06</v>
       </c>
       <c r="C45" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E45" s="5" t="s">
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" t="s">
         <v>22</v>
       </c>
       <c r="G45" t="s">
         <v>23</v>
       </c>
-      <c r="I45" s="5" t="s">
-        <v>59</v>
+      <c r="I45" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46">
+        <v>0.45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" t="s">
+        <v>59</v>
+      </c>
+      <c r="G46" t="s">
+        <v>23</v>
+      </c>
+      <c r="I46" t="s">
         <v>60</v>
-      </c>
-      <c r="B46" s="5">
-        <v>0.45</v>
-      </c>
-      <c r="C46" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" s="5">
+        <v>61</v>
+      </c>
+      <c r="B47">
         <v>0.9</v>
       </c>
       <c r="C47" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" t="s">
         <v>22</v>
       </c>
       <c r="G47" t="s">
         <v>23</v>
       </c>
-      <c r="I47" s="5" t="s">
-        <v>64</v>
+      <c r="I47" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48">
         <v>0.9</v>
       </c>
       <c r="C48" t="s">
@@ -1770,7 +1762,7 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1794,7 +1786,7 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1810,7 +1802,7 @@
         <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1818,7 +1810,7 @@
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1858,26 +1850,26 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
-        <v>172</v>
+      <c r="A60" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D60" t="s">
         <v>42</v>
       </c>
       <c r="E60" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F60" t="s">
         <v>19</v>
       </c>
       <c r="G60" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1905,7 +1897,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B62">
         <v>-2700</v>
@@ -1914,7 +1906,7 @@
         <v>21</v>
       </c>
       <c r="D62" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E62" t="s">
         <v>22</v>
@@ -1923,12 +1915,12 @@
         <v>23</v>
       </c>
       <c r="G62" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B63">
         <v>120000</v>
@@ -1946,7 +1938,7 @@
         <v>23</v>
       </c>
       <c r="G63" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1974,7 +1966,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B65">
         <v>0.56999999999999995</v>
@@ -1992,12 +1984,12 @@
         <v>23</v>
       </c>
       <c r="G65" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B66">
         <v>15.3</v>
@@ -2015,12 +2007,12 @@
         <v>23</v>
       </c>
       <c r="G66" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B67">
         <v>5340</v>
@@ -2038,12 +2030,12 @@
         <v>23</v>
       </c>
       <c r="G67" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B68">
         <v>1200</v>
@@ -2055,18 +2047,18 @@
         <v>42</v>
       </c>
       <c r="E68" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F68" t="s">
         <v>23</v>
       </c>
       <c r="G68" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B69">
         <v>9000</v>
@@ -2078,24 +2070,24 @@
         <v>42</v>
       </c>
       <c r="E69" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F69" t="s">
         <v>23</v>
       </c>
       <c r="G69" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B70">
         <v>118</v>
       </c>
       <c r="C70" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D70" t="s">
         <v>42</v>
@@ -2107,12 +2099,12 @@
         <v>23</v>
       </c>
       <c r="G70" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B71">
         <v>1070</v>
@@ -2121,21 +2113,21 @@
         <v>21</v>
       </c>
       <c r="D71" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" t="s">
+        <v>82</v>
+      </c>
+      <c r="F71" t="s">
+        <v>23</v>
+      </c>
+      <c r="G71" t="s">
         <v>83</v>
-      </c>
-      <c r="E71" t="s">
-        <v>84</v>
-      </c>
-      <c r="F71" t="s">
-        <v>23</v>
-      </c>
-      <c r="G71" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B72">
         <v>6580</v>
@@ -2147,18 +2139,18 @@
         <v>42</v>
       </c>
       <c r="E72" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F72" t="s">
         <v>23</v>
       </c>
       <c r="G72" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B73">
         <f>0.6/250</f>
@@ -2171,24 +2163,21 @@
         <v>42</v>
       </c>
       <c r="E73" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F73" t="s">
         <v>23</v>
       </c>
       <c r="G73" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -2212,7 +2201,7 @@
         <v>4</v>
       </c>
       <c r="B78" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -2228,7 +2217,7 @@
         <v>7</v>
       </c>
       <c r="B80" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -2236,7 +2225,7 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -2276,26 +2265,26 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
-        <v>173</v>
+      <c r="A85" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="B85">
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D85" t="s">
         <v>42</v>
       </c>
       <c r="E85" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F85" t="s">
         <v>19</v>
       </c>
       <c r="G85" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -2323,7 +2312,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B87">
         <v>-10900</v>
@@ -2332,7 +2321,7 @@
         <v>21</v>
       </c>
       <c r="D87" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E87" t="s">
         <v>22</v>
@@ -2341,12 +2330,12 @@
         <v>23</v>
       </c>
       <c r="G87" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B88">
         <v>225000</v>
@@ -2364,7 +2353,7 @@
         <v>23</v>
       </c>
       <c r="G88" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -2392,7 +2381,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B90">
         <v>1.9</v>
@@ -2410,12 +2399,12 @@
         <v>23</v>
       </c>
       <c r="G90" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B91">
         <v>51.1</v>
@@ -2433,12 +2422,12 @@
         <v>23</v>
       </c>
       <c r="G91" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B92">
         <v>21800</v>
@@ -2456,12 +2445,12 @@
         <v>23</v>
       </c>
       <c r="G92" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B93">
         <v>1200</v>
@@ -2473,18 +2462,18 @@
         <v>42</v>
       </c>
       <c r="E93" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F93" t="s">
         <v>23</v>
       </c>
       <c r="G93" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B94">
         <v>9000</v>
@@ -2496,24 +2485,24 @@
         <v>42</v>
       </c>
       <c r="E94" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F94" t="s">
         <v>23</v>
       </c>
       <c r="G94" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B95">
         <v>35</v>
       </c>
       <c r="C95" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D95" t="s">
         <v>42</v>
@@ -2525,12 +2514,12 @@
         <v>23</v>
       </c>
       <c r="G95" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B96">
         <v>13600</v>
@@ -2539,21 +2528,21 @@
         <v>21</v>
       </c>
       <c r="D96" t="s">
+        <v>81</v>
+      </c>
+      <c r="E96" t="s">
+        <v>82</v>
+      </c>
+      <c r="F96" t="s">
+        <v>23</v>
+      </c>
+      <c r="G96" t="s">
         <v>83</v>
-      </c>
-      <c r="E96" t="s">
-        <v>84</v>
-      </c>
-      <c r="F96" t="s">
-        <v>23</v>
-      </c>
-      <c r="G96" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B97">
         <v>4390</v>
@@ -2565,18 +2554,18 @@
         <v>42</v>
       </c>
       <c r="E97" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F97" t="s">
         <v>23</v>
       </c>
       <c r="G97" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B98">
         <f>0.6/250</f>
@@ -2589,24 +2578,21 @@
         <v>42</v>
       </c>
       <c r="E98" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F98" t="s">
         <v>23</v>
       </c>
       <c r="G98" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="100" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -2630,7 +2616,7 @@
         <v>4</v>
       </c>
       <c r="B103" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -2654,7 +2640,7 @@
         <v>10</v>
       </c>
       <c r="B106" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -2697,14 +2683,14 @@
       </c>
     </row>
     <row r="110" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
-        <v>81</v>
+      <c r="A110" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B110">
         <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D110" t="s">
         <v>42</v>
@@ -2716,12 +2702,12 @@
         <v>19</v>
       </c>
       <c r="H110" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
-        <v>182</v>
+      <c r="A111" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="B111">
         <v>-1.4E-5</v>
@@ -2739,12 +2725,12 @@
         <v>23</v>
       </c>
       <c r="H111" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
-        <v>178</v>
+      <c r="A112" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="B112">
         <v>-1.6000000000000001E-4</v>
@@ -2753,7 +2739,7 @@
         <v>21</v>
       </c>
       <c r="D112" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F112" t="s">
         <v>22</v>
@@ -2762,12 +2748,12 @@
         <v>23</v>
       </c>
       <c r="H112" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" s="14" t="s">
-        <v>180</v>
+      <c r="A113" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="B113">
         <v>-9.0600000000000007E-5</v>
@@ -2785,12 +2771,12 @@
         <v>23</v>
       </c>
       <c r="H113" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
-        <v>86</v>
+      <c r="A114" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="B114">
         <v>0.2</v>
@@ -2799,7 +2785,7 @@
         <v>21</v>
       </c>
       <c r="D114" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F114" t="s">
         <v>22</v>
@@ -2807,13 +2793,13 @@
       <c r="G114" t="s">
         <v>23</v>
       </c>
-      <c r="H114" s="4" t="s">
-        <v>87</v>
+      <c r="H114" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115" s="4" t="s">
-        <v>88</v>
+      <c r="A115" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="B115">
         <v>1.5E-3</v>
@@ -2831,35 +2817,35 @@
         <v>23</v>
       </c>
       <c r="H115" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B116" s="5">
+        <v>9.0599999999999999E-7</v>
+      </c>
+      <c r="C116" t="s">
+        <v>21</v>
+      </c>
+      <c r="D116" t="s">
+        <v>42</v>
+      </c>
+      <c r="F116" t="s">
+        <v>22</v>
+      </c>
+      <c r="G116" t="s">
+        <v>23</v>
+      </c>
+      <c r="H116" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="s">
+    <row r="117" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="B116" s="11">
-        <v>9.0599999999999999E-7</v>
-      </c>
-      <c r="C116" t="s">
-        <v>21</v>
-      </c>
-      <c r="D116" t="s">
-        <v>42</v>
-      </c>
-      <c r="F116" t="s">
-        <v>22</v>
-      </c>
-      <c r="G116" t="s">
-        <v>23</v>
-      </c>
-      <c r="H116" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="B117">
         <v>3.5999999999999994E-5</v>
@@ -2877,12 +2863,12 @@
         <v>23</v>
       </c>
       <c r="H117" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" s="4" t="s">
-        <v>94</v>
+      <c r="A118" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B118">
         <v>0.76800000000000002</v>
@@ -2891,21 +2877,21 @@
         <v>21</v>
       </c>
       <c r="D118" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F118" t="s">
+        <v>93</v>
+      </c>
+      <c r="G118" t="s">
+        <v>23</v>
+      </c>
+      <c r="H118" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="G118" t="s">
-        <v>23</v>
-      </c>
-      <c r="H118" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="B119">
         <v>2.01E-2</v>
@@ -2917,18 +2903,18 @@
         <v>42</v>
       </c>
       <c r="F119" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G119" t="s">
         <v>23</v>
       </c>
       <c r="H119" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="4" t="s">
-        <v>99</v>
+      <c r="A120" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="B120">
         <v>2.2200000000000001E-2</v>
@@ -2946,12 +2932,12 @@
         <v>23</v>
       </c>
       <c r="H120" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" s="4" t="s">
-        <v>101</v>
+      <c r="A121" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="B121">
         <v>0.76800000000000002</v>
@@ -2960,23 +2946,23 @@
         <v>21</v>
       </c>
       <c r="D121" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F121" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G121" t="s">
         <v>23</v>
       </c>
       <c r="H121" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B122" s="11">
+      <c r="A122" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B122" s="5">
         <v>1.6300000000000001E-13</v>
       </c>
       <c r="C122" t="s">
@@ -2992,12 +2978,12 @@
         <v>23</v>
       </c>
       <c r="H122" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="4" t="s">
-        <v>105</v>
+      <c r="A123" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -3015,12 +3001,12 @@
         <v>23</v>
       </c>
       <c r="H123" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="4" t="s">
-        <v>107</v>
+      <c r="A124" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="B124">
         <v>3.8000000000000002E-4</v>
@@ -3038,12 +3024,12 @@
         <v>23</v>
       </c>
       <c r="H124" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="4" t="s">
-        <v>187</v>
+      <c r="A125" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="B125">
         <v>8.0399999999999985E-3</v>
@@ -3055,476 +3041,476 @@
         <v>42</v>
       </c>
       <c r="F125" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G125" t="s">
         <v>23</v>
       </c>
       <c r="H125" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B126" s="6">
+        <v>2.0333333333333332E-2</v>
+      </c>
+      <c r="C126" t="s">
+        <v>21</v>
+      </c>
+      <c r="D126" t="s">
+        <v>42</v>
+      </c>
+      <c r="F126" t="s">
+        <v>59</v>
+      </c>
+      <c r="G126" t="s">
+        <v>23</v>
+      </c>
+      <c r="H126" t="s">
         <v>60</v>
       </c>
-      <c r="B126" s="12">
-        <v>2.0333333333333332E-2</v>
-      </c>
-      <c r="C126" t="s">
-        <v>21</v>
-      </c>
-      <c r="D126" t="s">
-        <v>42</v>
-      </c>
-      <c r="F126" t="s">
-        <v>61</v>
-      </c>
-      <c r="G126" t="s">
-        <v>23</v>
-      </c>
-      <c r="H126" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="127" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A127" s="4" t="s">
-        <v>109</v>
+      <c r="A127" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="B127">
         <v>4.3600000000000003E-5</v>
       </c>
       <c r="C127" t="s">
+        <v>108</v>
+      </c>
+      <c r="E127" t="s">
+        <v>109</v>
+      </c>
+      <c r="F127" t="s">
+        <v>22</v>
+      </c>
+      <c r="G127" t="s">
         <v>110</v>
       </c>
-      <c r="E127" t="s">
+    </row>
+    <row r="128" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="F127" t="s">
-        <v>22</v>
-      </c>
-      <c r="G127" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A128" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="B128">
         <v>1.9000000000000002E-10</v>
       </c>
       <c r="C128" t="s">
+        <v>108</v>
+      </c>
+      <c r="E128" t="s">
+        <v>109</v>
+      </c>
+      <c r="F128" t="s">
+        <v>22</v>
+      </c>
+      <c r="G128" t="s">
         <v>110</v>
       </c>
-      <c r="E128" t="s">
-        <v>111</v>
-      </c>
-      <c r="F128" t="s">
-        <v>22</v>
-      </c>
-      <c r="G128" t="s">
+    </row>
+    <row r="129" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A129" s="3" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="B129">
         <v>1.3200000000000001E-5</v>
       </c>
       <c r="C129" t="s">
+        <v>108</v>
+      </c>
+      <c r="E129" t="s">
+        <v>113</v>
+      </c>
+      <c r="F129" t="s">
+        <v>22</v>
+      </c>
+      <c r="G129" t="s">
         <v>110</v>
       </c>
-      <c r="E129" t="s">
+    </row>
+    <row r="130" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A130" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B130" s="5">
+        <v>1.31E-9</v>
+      </c>
+      <c r="C130" t="s">
+        <v>108</v>
+      </c>
+      <c r="E130" t="s">
+        <v>109</v>
+      </c>
+      <c r="F130" t="s">
+        <v>22</v>
+      </c>
+      <c r="G130" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A131" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="F129" t="s">
-        <v>22</v>
-      </c>
-      <c r="G129" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A130" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B130" s="11">
-        <v>1.31E-9</v>
-      </c>
-      <c r="C130" t="s">
-        <v>110</v>
-      </c>
-      <c r="E130" t="s">
-        <v>111</v>
-      </c>
-      <c r="F130" t="s">
-        <v>22</v>
-      </c>
-      <c r="G130" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="B131">
         <v>1.3200000000000001E-4</v>
       </c>
       <c r="C131" t="s">
+        <v>108</v>
+      </c>
+      <c r="E131" t="s">
+        <v>113</v>
+      </c>
+      <c r="F131" t="s">
+        <v>22</v>
+      </c>
+      <c r="G131" t="s">
         <v>110</v>
       </c>
-      <c r="E131" t="s">
-        <v>115</v>
-      </c>
-      <c r="F131" t="s">
-        <v>22</v>
-      </c>
-      <c r="G131" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="132" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A132" s="4" t="s">
-        <v>118</v>
+      <c r="A132" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="B132">
         <v>1.88E-6</v>
       </c>
       <c r="C132" t="s">
+        <v>108</v>
+      </c>
+      <c r="E132" t="s">
+        <v>113</v>
+      </c>
+      <c r="F132" t="s">
+        <v>22</v>
+      </c>
+      <c r="G132" t="s">
         <v>110</v>
       </c>
-      <c r="E132" t="s">
-        <v>115</v>
-      </c>
-      <c r="F132" t="s">
-        <v>22</v>
-      </c>
-      <c r="G132" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="133" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A133" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B133" s="11">
+      <c r="A133" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B133" s="5">
         <v>7.6000000000000002E-9</v>
       </c>
       <c r="C133" t="s">
+        <v>108</v>
+      </c>
+      <c r="E133" t="s">
+        <v>113</v>
+      </c>
+      <c r="F133" t="s">
+        <v>22</v>
+      </c>
+      <c r="G133" t="s">
         <v>110</v>
       </c>
-      <c r="E133" t="s">
-        <v>115</v>
-      </c>
-      <c r="F133" t="s">
-        <v>22</v>
-      </c>
-      <c r="G133" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="134" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A134" s="4" t="s">
-        <v>120</v>
+      <c r="A134" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="B134">
         <v>1.5699999999999999E-4</v>
       </c>
       <c r="C134" t="s">
+        <v>108</v>
+      </c>
+      <c r="E134" t="s">
+        <v>109</v>
+      </c>
+      <c r="F134" t="s">
+        <v>22</v>
+      </c>
+      <c r="G134" t="s">
         <v>110</v>
       </c>
-      <c r="E134" t="s">
-        <v>111</v>
-      </c>
-      <c r="F134" t="s">
-        <v>22</v>
-      </c>
-      <c r="G134" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="135" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A135" s="4" t="s">
-        <v>121</v>
+      <c r="A135" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="B135">
         <v>7.62E-3</v>
       </c>
       <c r="C135" t="s">
+        <v>108</v>
+      </c>
+      <c r="E135" t="s">
+        <v>109</v>
+      </c>
+      <c r="F135" t="s">
+        <v>22</v>
+      </c>
+      <c r="G135" t="s">
         <v>110</v>
       </c>
-      <c r="E135" t="s">
-        <v>111</v>
-      </c>
-      <c r="F135" t="s">
-        <v>22</v>
-      </c>
-      <c r="G135" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="136" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A136" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B136" s="11">
+      <c r="A136" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B136" s="5">
         <v>1.1900000000000001E-7</v>
       </c>
       <c r="C136" t="s">
+        <v>108</v>
+      </c>
+      <c r="E136" t="s">
+        <v>113</v>
+      </c>
+      <c r="F136" t="s">
+        <v>22</v>
+      </c>
+      <c r="G136" t="s">
         <v>110</v>
       </c>
-      <c r="E136" t="s">
-        <v>115</v>
-      </c>
-      <c r="F136" t="s">
-        <v>22</v>
-      </c>
-      <c r="G136" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="137" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A137" s="4" t="s">
-        <v>123</v>
+      <c r="A137" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="B137">
         <v>1.8300000000000001E-5</v>
       </c>
       <c r="C137" t="s">
+        <v>108</v>
+      </c>
+      <c r="E137" t="s">
+        <v>109</v>
+      </c>
+      <c r="F137" t="s">
+        <v>22</v>
+      </c>
+      <c r="G137" t="s">
         <v>110</v>
       </c>
-      <c r="E137" t="s">
-        <v>111</v>
-      </c>
-      <c r="F137" t="s">
-        <v>22</v>
-      </c>
-      <c r="G137" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="138" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A138" s="4" t="s">
-        <v>124</v>
+      <c r="A138" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="B138">
         <v>1.3999999999999999E-6</v>
       </c>
       <c r="C138" t="s">
+        <v>108</v>
+      </c>
+      <c r="E138" t="s">
+        <v>109</v>
+      </c>
+      <c r="F138" t="s">
+        <v>22</v>
+      </c>
+      <c r="G138" t="s">
         <v>110</v>
       </c>
-      <c r="E138" t="s">
-        <v>111</v>
-      </c>
-      <c r="F138" t="s">
-        <v>22</v>
-      </c>
-      <c r="G138" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="139" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A139" s="4" t="s">
-        <v>124</v>
+      <c r="A139" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="B139">
         <v>5.6499999999999993E-6</v>
       </c>
       <c r="C139" t="s">
+        <v>108</v>
+      </c>
+      <c r="E139" t="s">
+        <v>113</v>
+      </c>
+      <c r="F139" t="s">
+        <v>22</v>
+      </c>
+      <c r="G139" t="s">
         <v>110</v>
       </c>
-      <c r="E139" t="s">
-        <v>115</v>
-      </c>
-      <c r="F139" t="s">
-        <v>22</v>
-      </c>
-      <c r="G139" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="140" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A140" s="4" t="s">
+      <c r="A140" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B140" s="5">
+        <v>3.4000000000000003E-9</v>
+      </c>
+      <c r="C140" t="s">
+        <v>108</v>
+      </c>
+      <c r="E140" t="s">
+        <v>109</v>
+      </c>
+      <c r="F140" t="s">
+        <v>22</v>
+      </c>
+      <c r="G140" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A141" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B141" s="5">
+        <v>1.51E-9</v>
+      </c>
+      <c r="C141" t="s">
+        <v>108</v>
+      </c>
+      <c r="E141" t="s">
+        <v>113</v>
+      </c>
+      <c r="F141" t="s">
+        <v>22</v>
+      </c>
+      <c r="G141" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A142" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B142" s="5">
+        <v>9.9999999999999986E-10</v>
+      </c>
+      <c r="C142" t="s">
+        <v>108</v>
+      </c>
+      <c r="E142" t="s">
+        <v>113</v>
+      </c>
+      <c r="F142" t="s">
+        <v>22</v>
+      </c>
+      <c r="G142" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A143" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B140" s="11">
-        <v>3.4000000000000003E-9</v>
-      </c>
-      <c r="C140" t="s">
+      <c r="B143" s="5">
+        <v>1.0399999999999999E-7</v>
+      </c>
+      <c r="C143" t="s">
+        <v>108</v>
+      </c>
+      <c r="E143" t="s">
+        <v>113</v>
+      </c>
+      <c r="F143" t="s">
+        <v>22</v>
+      </c>
+      <c r="G143" t="s">
         <v>110</v>
       </c>
-      <c r="E140" t="s">
-        <v>111</v>
-      </c>
-      <c r="F140" t="s">
-        <v>22</v>
-      </c>
-      <c r="G140" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A141" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B141" s="11">
-        <v>1.51E-9</v>
-      </c>
-      <c r="C141" t="s">
+    </row>
+    <row r="144" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A144" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B144" s="5">
+        <v>9.0000000000000012E-8</v>
+      </c>
+      <c r="C144" t="s">
+        <v>108</v>
+      </c>
+      <c r="E144" t="s">
+        <v>113</v>
+      </c>
+      <c r="F144" t="s">
+        <v>22</v>
+      </c>
+      <c r="G144" t="s">
         <v>110</v>
       </c>
-      <c r="E141" t="s">
-        <v>115</v>
-      </c>
-      <c r="F141" t="s">
-        <v>22</v>
-      </c>
-      <c r="G141" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A142" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B142" s="11">
-        <v>9.9999999999999986E-10</v>
-      </c>
-      <c r="C142" t="s">
+    </row>
+    <row r="145" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A145" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B145" s="5">
+        <v>2.2399999999999999E-7</v>
+      </c>
+      <c r="C145" t="s">
+        <v>108</v>
+      </c>
+      <c r="E145" t="s">
+        <v>113</v>
+      </c>
+      <c r="F145" t="s">
+        <v>22</v>
+      </c>
+      <c r="G145" t="s">
         <v>110</v>
       </c>
-      <c r="E142" t="s">
-        <v>115</v>
-      </c>
-      <c r="F142" t="s">
-        <v>22</v>
-      </c>
-      <c r="G142" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A143" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B143" s="11">
-        <v>1.0399999999999999E-7</v>
-      </c>
-      <c r="C143" t="s">
+    </row>
+    <row r="146" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A146" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B146" s="5">
+        <v>2.9700000000000003E-7</v>
+      </c>
+      <c r="C146" t="s">
+        <v>108</v>
+      </c>
+      <c r="E146" t="s">
+        <v>113</v>
+      </c>
+      <c r="F146" t="s">
+        <v>22</v>
+      </c>
+      <c r="G146" t="s">
         <v>110</v>
       </c>
-      <c r="E143" t="s">
-        <v>115</v>
-      </c>
-      <c r="F143" t="s">
-        <v>22</v>
-      </c>
-      <c r="G143" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A144" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B144" s="11">
-        <v>9.0000000000000012E-8</v>
-      </c>
-      <c r="C144" t="s">
+    </row>
+    <row r="147" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A147" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B147" s="5">
+        <v>2.7500000000000001E-5</v>
+      </c>
+      <c r="C147" t="s">
+        <v>108</v>
+      </c>
+      <c r="E147" t="s">
+        <v>109</v>
+      </c>
+      <c r="F147" t="s">
+        <v>22</v>
+      </c>
+      <c r="G147" t="s">
         <v>110</v>
       </c>
-      <c r="E144" t="s">
-        <v>115</v>
-      </c>
-      <c r="F144" t="s">
-        <v>22</v>
-      </c>
-      <c r="G144" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A145" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B145" s="11">
-        <v>2.2399999999999999E-7</v>
-      </c>
-      <c r="C145" t="s">
+    </row>
+    <row r="148" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A148" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B148" s="5">
+        <v>1.9E-6</v>
+      </c>
+      <c r="C148" t="s">
+        <v>108</v>
+      </c>
+      <c r="E148" t="s">
+        <v>113</v>
+      </c>
+      <c r="F148" t="s">
+        <v>22</v>
+      </c>
+      <c r="G148" t="s">
         <v>110</v>
-      </c>
-      <c r="E145" t="s">
-        <v>115</v>
-      </c>
-      <c r="F145" t="s">
-        <v>22</v>
-      </c>
-      <c r="G145" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A146" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B146" s="11">
-        <v>2.9700000000000003E-7</v>
-      </c>
-      <c r="C146" t="s">
-        <v>110</v>
-      </c>
-      <c r="E146" t="s">
-        <v>115</v>
-      </c>
-      <c r="F146" t="s">
-        <v>22</v>
-      </c>
-      <c r="G146" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A147" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B147" s="11">
-        <v>2.7500000000000001E-5</v>
-      </c>
-      <c r="C147" t="s">
-        <v>110</v>
-      </c>
-      <c r="E147" t="s">
-        <v>111</v>
-      </c>
-      <c r="F147" t="s">
-        <v>22</v>
-      </c>
-      <c r="G147" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A148" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B148" s="11">
-        <v>1.9E-6</v>
-      </c>
-      <c r="C148" t="s">
-        <v>110</v>
-      </c>
-      <c r="E148" t="s">
-        <v>115</v>
-      </c>
-      <c r="F148" t="s">
-        <v>22</v>
-      </c>
-      <c r="G148" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3532,7 +3518,7 @@
         <v>0</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -3556,7 +3542,7 @@
         <v>4</v>
       </c>
       <c r="B153" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -3580,7 +3566,7 @@
         <v>10</v>
       </c>
       <c r="B156" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
@@ -3623,14 +3609,14 @@
       </c>
     </row>
     <row r="160" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A160" s="4" t="s">
-        <v>136</v>
+      <c r="A160" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="B160">
         <v>1</v>
       </c>
       <c r="C160" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D160" t="s">
         <v>42</v>
@@ -3642,14 +3628,14 @@
         <v>19</v>
       </c>
       <c r="H160" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A161" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="B161" s="11">
+      <c r="A161" t="s">
+        <v>142</v>
+      </c>
+      <c r="B161" s="5">
         <v>1.61E-7</v>
       </c>
       <c r="C161" t="s">
@@ -3665,37 +3651,37 @@
         <v>23</v>
       </c>
       <c r="H161" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="162" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A162" s="6" t="s">
+      <c r="A162" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B162" s="5">
+        <v>3.1999999999999999E-5</v>
+      </c>
+      <c r="C162" t="s">
+        <v>21</v>
+      </c>
+      <c r="D162" t="s">
+        <v>140</v>
+      </c>
+      <c r="F162" t="s">
+        <v>22</v>
+      </c>
+      <c r="G162" t="s">
+        <v>23</v>
+      </c>
+      <c r="H162" t="s">
         <v>141</v>
       </c>
-      <c r="B162" s="11">
-        <v>3.1999999999999999E-5</v>
-      </c>
-      <c r="C162" t="s">
-        <v>21</v>
-      </c>
-      <c r="D162" t="s">
-        <v>142</v>
-      </c>
-      <c r="F162" t="s">
-        <v>22</v>
-      </c>
-      <c r="G162" t="s">
-        <v>23</v>
-      </c>
-      <c r="H162" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A163" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B163" s="11">
+      <c r="A163" t="s">
+        <v>137</v>
+      </c>
+      <c r="B163" s="5">
         <v>3.2000000000000003E-4</v>
       </c>
       <c r="C163" t="s">
@@ -3711,14 +3697,14 @@
         <v>23</v>
       </c>
       <c r="H163" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A164" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B164" s="11">
+      <c r="A164" t="s">
+        <v>146</v>
+      </c>
+      <c r="B164" s="5">
         <v>0.16600000000000001</v>
       </c>
       <c r="C164" t="s">
@@ -3734,30 +3720,30 @@
         <v>23</v>
       </c>
       <c r="H164" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A165" s="7" t="s">
+      <c r="A165" t="s">
+        <v>58</v>
+      </c>
+      <c r="B165" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="C165" t="s">
+        <v>21</v>
+      </c>
+      <c r="D165" t="s">
+        <v>42</v>
+      </c>
+      <c r="F165" t="s">
+        <v>59</v>
+      </c>
+      <c r="G165" t="s">
+        <v>23</v>
+      </c>
+      <c r="H165" t="s">
         <v>60</v>
-      </c>
-      <c r="B165" s="11">
-        <v>0.66</v>
-      </c>
-      <c r="C165" t="s">
-        <v>21</v>
-      </c>
-      <c r="D165" t="s">
-        <v>42</v>
-      </c>
-      <c r="F165" t="s">
-        <v>61</v>
-      </c>
-      <c r="G165" t="s">
-        <v>23</v>
-      </c>
-      <c r="H165" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="167" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3765,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
@@ -3789,7 +3775,7 @@
         <v>4</v>
       </c>
       <c r="B170" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
@@ -3813,7 +3799,7 @@
         <v>10</v>
       </c>
       <c r="B173" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
@@ -3856,14 +3842,14 @@
       </c>
     </row>
     <row r="177" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A177" s="4" t="s">
-        <v>146</v>
+      <c r="A177" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="B177">
         <v>1</v>
       </c>
       <c r="C177" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D177" t="s">
         <v>42</v>
@@ -3875,14 +3861,14 @@
         <v>19</v>
       </c>
       <c r="H177" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A178" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="B178" s="11">
+      <c r="A178" t="s">
+        <v>142</v>
+      </c>
+      <c r="B178" s="5">
         <v>1.61E-7</v>
       </c>
       <c r="C178" t="s">
@@ -3898,37 +3884,37 @@
         <v>23</v>
       </c>
       <c r="H178" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A179" s="6" t="s">
+      <c r="A179" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B179" s="5">
+        <v>3.1999999999999999E-5</v>
+      </c>
+      <c r="C179" t="s">
+        <v>21</v>
+      </c>
+      <c r="D179" t="s">
+        <v>140</v>
+      </c>
+      <c r="F179" t="s">
+        <v>22</v>
+      </c>
+      <c r="G179" t="s">
+        <v>23</v>
+      </c>
+      <c r="H179" t="s">
         <v>141</v>
       </c>
-      <c r="B179" s="11">
-        <v>3.1999999999999999E-5</v>
-      </c>
-      <c r="C179" t="s">
-        <v>21</v>
-      </c>
-      <c r="D179" t="s">
-        <v>142</v>
-      </c>
-      <c r="F179" t="s">
-        <v>22</v>
-      </c>
-      <c r="G179" t="s">
-        <v>23</v>
-      </c>
-      <c r="H179" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A180" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B180" s="11">
+      <c r="A180" t="s">
+        <v>137</v>
+      </c>
+      <c r="B180" s="5">
         <v>3.2000000000000003E-4</v>
       </c>
       <c r="C180" t="s">
@@ -3944,14 +3930,14 @@
         <v>23</v>
       </c>
       <c r="H180" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A181" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B181" s="11">
+      <c r="A181" t="s">
+        <v>146</v>
+      </c>
+      <c r="B181" s="5">
         <v>0.16600000000000001</v>
       </c>
       <c r="C181" t="s">
@@ -3967,35 +3953,35 @@
         <v>23</v>
       </c>
       <c r="H181" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A182" s="7" t="s">
+      <c r="A182" t="s">
+        <v>58</v>
+      </c>
+      <c r="B182" s="5">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="C182" t="s">
+        <v>21</v>
+      </c>
+      <c r="D182" t="s">
+        <v>42</v>
+      </c>
+      <c r="F182" t="s">
+        <v>59</v>
+      </c>
+      <c r="G182" t="s">
+        <v>23</v>
+      </c>
+      <c r="H182" t="s">
         <v>60</v>
       </c>
-      <c r="B182" s="11">
-        <v>0.36599999999999999</v>
-      </c>
-      <c r="C182" t="s">
-        <v>21</v>
-      </c>
-      <c r="D182" t="s">
-        <v>42</v>
-      </c>
-      <c r="F182" t="s">
-        <v>61</v>
-      </c>
-      <c r="G182" t="s">
-        <v>23</v>
-      </c>
-      <c r="H182" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A183" s="5" t="s">
-        <v>97</v>
+      <c r="A183" t="s">
+        <v>95</v>
       </c>
       <c r="B183">
         <f>9.5*3.6</f>
@@ -4008,13 +3994,13 @@
         <v>42</v>
       </c>
       <c r="F183" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G183" t="s">
         <v>23</v>
       </c>
       <c r="H183" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4022,7 +4008,7 @@
         <v>0</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
@@ -4046,7 +4032,7 @@
         <v>4</v>
       </c>
       <c r="B188" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
@@ -4070,7 +4056,7 @@
         <v>10</v>
       </c>
       <c r="B191" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
@@ -4113,10 +4099,10 @@
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A195" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B195" s="13">
+      <c r="A195" t="s">
+        <v>146</v>
+      </c>
+      <c r="B195" s="7">
         <v>1</v>
       </c>
       <c r="C195" t="s">
@@ -4132,12 +4118,12 @@
         <v>19</v>
       </c>
       <c r="H195" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A196" s="7" t="s">
-        <v>150</v>
+      <c r="A196" t="s">
+        <v>148</v>
       </c>
       <c r="B196">
         <v>1.2</v>
@@ -4146,7 +4132,7 @@
         <v>21</v>
       </c>
       <c r="D196" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F196" t="s">
         <v>22</v>
@@ -4154,13 +4140,13 @@
       <c r="G196" t="s">
         <v>23</v>
       </c>
-      <c r="H196" s="7" t="s">
-        <v>151</v>
+      <c r="H196" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A197" s="7" t="s">
-        <v>152</v>
+      <c r="A197" t="s">
+        <v>150</v>
       </c>
       <c r="B197">
         <v>1.03</v>
@@ -4177,13 +4163,13 @@
       <c r="G197" t="s">
         <v>23</v>
       </c>
-      <c r="H197" s="7" t="s">
-        <v>153</v>
+      <c r="H197" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A198" s="7" t="s">
-        <v>154</v>
+      <c r="A198" t="s">
+        <v>152</v>
       </c>
       <c r="B198">
         <v>0.26</v>
@@ -4200,15 +4186,15 @@
       <c r="G198" t="s">
         <v>23</v>
       </c>
-      <c r="H198" s="7" t="s">
+      <c r="H198" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A199" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B199" s="11">
+      <c r="B199" s="5">
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="C199" t="s">
@@ -4223,13 +4209,13 @@
       <c r="G199" t="s">
         <v>23</v>
       </c>
-      <c r="H199" s="7" t="s">
-        <v>158</v>
+      <c r="H199" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A200" s="7" t="s">
-        <v>60</v>
+      <c r="A200" t="s">
+        <v>58</v>
       </c>
       <c r="B200">
         <v>42.1</v>
@@ -4241,18 +4227,18 @@
         <v>42</v>
       </c>
       <c r="F200" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G200" t="s">
         <v>23</v>
       </c>
       <c r="H200" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="201" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A201" s="4" t="s">
-        <v>97</v>
+      <c r="A201" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="B201">
         <v>2.7</v>
@@ -4264,18 +4250,18 @@
         <v>42</v>
       </c>
       <c r="F201" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G201" t="s">
         <v>23</v>
       </c>
       <c r="H201" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B202">
         <v>0.2</v>
@@ -4287,13 +4273,13 @@
         <v>42</v>
       </c>
       <c r="F202" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G202" t="s">
         <v>23</v>
       </c>
       <c r="H202" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="204" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4301,7 +4287,7 @@
         <v>0</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
@@ -4325,7 +4311,7 @@
         <v>4</v>
       </c>
       <c r="B207" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
@@ -4348,8 +4334,8 @@
       <c r="A210" t="s">
         <v>10</v>
       </c>
-      <c r="B210" s="7" t="s">
-        <v>161</v>
+      <c r="B210" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
@@ -4392,10 +4378,10 @@
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A214" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B214" s="13">
+      <c r="A214" t="s">
+        <v>160</v>
+      </c>
+      <c r="B214" s="7">
         <v>1</v>
       </c>
       <c r="C214" t="s">
@@ -4411,12 +4397,12 @@
         <v>19</v>
       </c>
       <c r="H214" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A215" s="7" t="s">
-        <v>60</v>
+      <c r="A215" t="s">
+        <v>58</v>
       </c>
       <c r="B215">
         <v>9.375E-2</v>
@@ -4428,18 +4414,18 @@
         <v>42</v>
       </c>
       <c r="F215" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G215" t="s">
         <v>23</v>
       </c>
       <c r="H215" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A216" s="7" t="s">
-        <v>159</v>
+      <c r="A216" t="s">
+        <v>157</v>
       </c>
       <c r="B216">
         <v>31.25</v>
@@ -4448,7 +4434,7 @@
         <v>21</v>
       </c>
       <c r="D216" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F216" t="s">
         <v>22</v>
@@ -4457,7 +4443,7 @@
         <v>23</v>
       </c>
       <c r="H216" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="218" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4465,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.2">
@@ -4489,7 +4475,7 @@
         <v>4</v>
       </c>
       <c r="B221" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.2">
@@ -4512,8 +4498,8 @@
       <c r="A224" t="s">
         <v>10</v>
       </c>
-      <c r="B224" s="7" t="s">
-        <v>165</v>
+      <c r="B224" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.2">
@@ -4556,10 +4542,10 @@
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A228" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B228" s="13">
+      <c r="A228" t="s">
+        <v>161</v>
+      </c>
+      <c r="B228" s="7">
         <v>1</v>
       </c>
       <c r="C228" t="s">
@@ -4575,12 +4561,12 @@
         <v>19</v>
       </c>
       <c r="H228" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A229" s="7" t="s">
-        <v>60</v>
+      <c r="A229" t="s">
+        <v>58</v>
       </c>
       <c r="B229">
         <v>0.34399999999999997</v>
@@ -4592,13 +4578,13 @@
         <v>42</v>
       </c>
       <c r="F229" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G229" t="s">
         <v>23</v>
       </c>
       <c r="H229" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="231" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4606,7 +4592,7 @@
         <v>0</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.2">
@@ -4630,7 +4616,7 @@
         <v>4</v>
       </c>
       <c r="B234" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.2">
@@ -4653,16 +4639,16 @@
       <c r="A237" t="s">
         <v>10</v>
       </c>
-      <c r="B237" s="7" t="s">
-        <v>169</v>
+      <c r="B237" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>8</v>
       </c>
-      <c r="B238" s="7" t="s">
-        <v>167</v>
+      <c r="B238" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="239" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4698,13 +4684,13 @@
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B241">
         <v>1</v>
       </c>
       <c r="C241" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D241" t="s">
         <v>42</v>
@@ -4716,12 +4702,12 @@
         <v>19</v>
       </c>
       <c r="H241" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A242" s="7" t="s">
-        <v>60</v>
+      <c r="A242" t="s">
+        <v>58</v>
       </c>
       <c r="B242">
         <v>2.46</v>
@@ -4733,18 +4719,18 @@
         <v>42</v>
       </c>
       <c r="F242" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G242" t="s">
         <v>23</v>
       </c>
       <c r="H242" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A243" s="7" t="s">
-        <v>170</v>
+      <c r="A243" t="s">
+        <v>168</v>
       </c>
       <c r="B243">
         <v>2.3999999999999998E-3</v>
@@ -4762,7 +4748,7 @@
         <v>23</v>
       </c>
       <c r="H243" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="245" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4770,7 +4756,7 @@
         <v>0</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.2">
@@ -4794,7 +4780,7 @@
         <v>4</v>
       </c>
       <c r="B248" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.2">
@@ -4810,7 +4796,7 @@
         <v>7</v>
       </c>
       <c r="B250" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.2">
@@ -4818,7 +4804,7 @@
         <v>10</v>
       </c>
       <c r="B251" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.2">
@@ -4858,31 +4844,31 @@
       </c>
     </row>
     <row r="255" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A255" s="4" t="s">
-        <v>174</v>
+      <c r="A255" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="B255">
         <v>1</v>
       </c>
       <c r="C255" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D255" t="s">
         <v>42</v>
       </c>
       <c r="E255" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F255" t="s">
         <v>19</v>
       </c>
       <c r="G255" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A256" s="7" t="s">
-        <v>60</v>
+      <c r="A256" t="s">
+        <v>58</v>
       </c>
       <c r="B256">
         <f>0.6/250</f>
@@ -4895,13 +4881,13 @@
         <v>42</v>
       </c>
       <c r="E256" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F256" t="s">
         <v>23</v>
       </c>
       <c r="G256" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="258" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -4909,7 +4895,7 @@
         <v>0</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.2">
@@ -4933,7 +4919,7 @@
         <v>4</v>
       </c>
       <c r="B261" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.2">
@@ -4949,7 +4935,7 @@
         <v>7</v>
       </c>
       <c r="B263" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.2">
@@ -4957,7 +4943,7 @@
         <v>10</v>
       </c>
       <c r="B264" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.2">
@@ -4997,31 +4983,31 @@
       </c>
     </row>
     <row r="268" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A268" s="4" t="s">
-        <v>176</v>
+      <c r="A268" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="B268">
         <v>1</v>
       </c>
       <c r="C268" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D268" t="s">
         <v>42</v>
       </c>
       <c r="E268" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F268" t="s">
         <v>19</v>
       </c>
       <c r="G268" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A269" s="7" t="s">
-        <v>60</v>
+      <c r="A269" t="s">
+        <v>58</v>
       </c>
       <c r="B269">
         <f>0.6/250</f>
@@ -5034,13 +5020,13 @@
         <v>42</v>
       </c>
       <c r="E269" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F269" t="s">
         <v>23</v>
       </c>
       <c r="G269" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix import of train LCIs
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-distribution.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-distribution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise_transport/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3FAA1F-1CD8-FA43-8809-8E082AF0BC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C19E01-C58B-FF41-9C6F-E9409D0A8FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="1600" windowWidth="27820" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="281">
   <si>
     <t>Activity</t>
   </si>
@@ -850,6 +850,66 @@
   </si>
   <si>
     <t>soda ash, light, crystalline, heptahydrate</t>
+  </si>
+  <si>
+    <t>Fuel tank, compressed hydrogen gas, 700bar, with aluminium liner</t>
+  </si>
+  <si>
+    <t>Hydrogen tank</t>
+  </si>
+  <si>
+    <t>worksheet name</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Evangelisti et al. 2017, doi: 10.1016/j.jclepro.2016.11.159</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>An aluminium lined hydrogen tank (Type III), weighting 93 kg per unit.</t>
+  </si>
+  <si>
+    <t>special remark</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>lci-pass_cars</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>energy storage</t>
+  </si>
+  <si>
+    <t>epoxy resin production, liquid</t>
+  </si>
+  <si>
+    <t>market for glass fibre</t>
+  </si>
+  <si>
+    <t>glass fibre</t>
+  </si>
+  <si>
+    <t>market for polyurethane, flexible foam</t>
+  </si>
+  <si>
+    <t>polyurethane, flexible foam</t>
+  </si>
+  <si>
+    <t>ENTSO-E</t>
+  </si>
+  <si>
+    <t>energy chain</t>
   </si>
 </sst>
 </file>
@@ -1237,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T382"/>
+  <dimension ref="A1:T406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="B197" sqref="B197"/>
+    <sheetView tabSelected="1" topLeftCell="A370" workbookViewId="0">
+      <selection activeCell="L398" sqref="L398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11304,6 +11364,418 @@
         <v>148</v>
       </c>
     </row>
+    <row r="384" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A384" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="385" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A385" t="s">
+        <v>1</v>
+      </c>
+      <c r="B385" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="386" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A386" t="s">
+        <v>3</v>
+      </c>
+      <c r="B386">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A387" t="s">
+        <v>4</v>
+      </c>
+      <c r="B387" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="388" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A388" t="s">
+        <v>5</v>
+      </c>
+      <c r="B388" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="389" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A389" t="s">
+        <v>7</v>
+      </c>
+      <c r="B389" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="390" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A390" t="s">
+        <v>263</v>
+      </c>
+      <c r="B390" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="391" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A391" t="s">
+        <v>8</v>
+      </c>
+      <c r="B391" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="392" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A392" t="s">
+        <v>266</v>
+      </c>
+      <c r="B392" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="393" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A393" t="s">
+        <v>268</v>
+      </c>
+      <c r="B393" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="394" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A394" t="s">
+        <v>10</v>
+      </c>
+      <c r="B394" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="395" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A395" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="396" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A396" t="s">
+        <v>13</v>
+      </c>
+      <c r="B396" t="s">
+        <v>14</v>
+      </c>
+      <c r="C396" t="s">
+        <v>15</v>
+      </c>
+      <c r="D396" t="s">
+        <v>1</v>
+      </c>
+      <c r="E396" t="s">
+        <v>7</v>
+      </c>
+      <c r="F396" t="s">
+        <v>16</v>
+      </c>
+      <c r="G396" t="s">
+        <v>5</v>
+      </c>
+      <c r="H396" t="s">
+        <v>4</v>
+      </c>
+      <c r="I396" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="397" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A397" t="s">
+        <v>160</v>
+      </c>
+      <c r="B397">
+        <v>0.21368817200000001</v>
+      </c>
+      <c r="C397" t="s">
+        <v>271</v>
+      </c>
+      <c r="D397" t="s">
+        <v>42</v>
+      </c>
+      <c r="E397" t="s">
+        <v>22</v>
+      </c>
+      <c r="F397" t="s">
+        <v>269</v>
+      </c>
+      <c r="G397" t="s">
+        <v>23</v>
+      </c>
+      <c r="H397" t="s">
+        <v>159</v>
+      </c>
+      <c r="I397" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="398" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A398" t="s">
+        <v>261</v>
+      </c>
+      <c r="B398">
+        <v>1</v>
+      </c>
+      <c r="C398" t="s">
+        <v>271</v>
+      </c>
+      <c r="D398" t="s">
+        <v>42</v>
+      </c>
+      <c r="E398" t="s">
+        <v>22</v>
+      </c>
+      <c r="F398" t="s">
+        <v>269</v>
+      </c>
+      <c r="G398" t="s">
+        <v>19</v>
+      </c>
+      <c r="H398" t="s">
+        <v>262</v>
+      </c>
+      <c r="I398" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="399" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A399" t="s">
+        <v>274</v>
+      </c>
+      <c r="B399">
+        <v>0.31989247300000001</v>
+      </c>
+      <c r="C399" t="s">
+        <v>271</v>
+      </c>
+      <c r="D399" t="s">
+        <v>42</v>
+      </c>
+      <c r="E399" t="s">
+        <v>22</v>
+      </c>
+      <c r="F399" t="s">
+        <v>269</v>
+      </c>
+      <c r="G399" t="s">
+        <v>23</v>
+      </c>
+      <c r="H399" t="s">
+        <v>57</v>
+      </c>
+      <c r="I399" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="400" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A400" t="s">
+        <v>37</v>
+      </c>
+      <c r="B400">
+        <v>0.45936559100000002</v>
+      </c>
+      <c r="C400" t="s">
+        <v>271</v>
+      </c>
+      <c r="D400" t="s">
+        <v>2</v>
+      </c>
+      <c r="E400" t="s">
+        <v>22</v>
+      </c>
+      <c r="F400" t="s">
+        <v>269</v>
+      </c>
+      <c r="G400" t="s">
+        <v>23</v>
+      </c>
+      <c r="H400" t="s">
+        <v>38</v>
+      </c>
+      <c r="I400" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="401" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A401" t="s">
+        <v>275</v>
+      </c>
+      <c r="B401">
+        <v>6.0139785000000001E-2</v>
+      </c>
+      <c r="C401" t="s">
+        <v>271</v>
+      </c>
+      <c r="D401" t="s">
+        <v>2</v>
+      </c>
+      <c r="E401" t="s">
+        <v>22</v>
+      </c>
+      <c r="F401" t="s">
+        <v>269</v>
+      </c>
+      <c r="G401" t="s">
+        <v>23</v>
+      </c>
+      <c r="H401" t="s">
+        <v>276</v>
+      </c>
+      <c r="I401" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="402" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A402" t="s">
+        <v>277</v>
+      </c>
+      <c r="B402">
+        <v>4.9903226000000002E-2</v>
+      </c>
+      <c r="C402" t="s">
+        <v>271</v>
+      </c>
+      <c r="D402" t="s">
+        <v>42</v>
+      </c>
+      <c r="E402" t="s">
+        <v>22</v>
+      </c>
+      <c r="F402" t="s">
+        <v>269</v>
+      </c>
+      <c r="G402" t="s">
+        <v>23</v>
+      </c>
+      <c r="H402" t="s">
+        <v>278</v>
+      </c>
+      <c r="I402" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="403" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A403" t="s">
+        <v>52</v>
+      </c>
+      <c r="B403">
+        <v>0.38387096799999998</v>
+      </c>
+      <c r="C403" t="s">
+        <v>271</v>
+      </c>
+      <c r="D403" t="s">
+        <v>2</v>
+      </c>
+      <c r="E403" t="s">
+        <v>22</v>
+      </c>
+      <c r="F403" t="s">
+        <v>269</v>
+      </c>
+      <c r="G403" t="s">
+        <v>23</v>
+      </c>
+      <c r="H403" t="s">
+        <v>53</v>
+      </c>
+      <c r="I403" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="404" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A404" t="s">
+        <v>27</v>
+      </c>
+      <c r="B404">
+        <v>0.11388172000000001</v>
+      </c>
+      <c r="C404" t="s">
+        <v>271</v>
+      </c>
+      <c r="D404" t="s">
+        <v>2</v>
+      </c>
+      <c r="E404" t="s">
+        <v>22</v>
+      </c>
+      <c r="F404" t="s">
+        <v>269</v>
+      </c>
+      <c r="G404" t="s">
+        <v>23</v>
+      </c>
+      <c r="H404" t="s">
+        <v>28</v>
+      </c>
+      <c r="I404" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="405" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A405" t="s">
+        <v>58</v>
+      </c>
+      <c r="B405">
+        <v>0.17658064500000001</v>
+      </c>
+      <c r="C405" t="s">
+        <v>271</v>
+      </c>
+      <c r="D405" t="s">
+        <v>279</v>
+      </c>
+      <c r="E405" t="s">
+        <v>59</v>
+      </c>
+      <c r="F405" t="s">
+        <v>269</v>
+      </c>
+      <c r="G405" t="s">
+        <v>23</v>
+      </c>
+      <c r="H405" t="s">
+        <v>60</v>
+      </c>
+      <c r="I405" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="406" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A406" t="s">
+        <v>30</v>
+      </c>
+      <c r="B406">
+        <v>0.11388172000000001</v>
+      </c>
+      <c r="C406" t="s">
+        <v>271</v>
+      </c>
+      <c r="D406" t="s">
+        <v>42</v>
+      </c>
+      <c r="E406" t="s">
+        <v>22</v>
+      </c>
+      <c r="F406" t="s">
+        <v>269</v>
+      </c>
+      <c r="G406" t="s">
+        <v>23</v>
+      </c>
+      <c r="H406" t="s">
+        <v>30</v>
+      </c>
+      <c r="I406" t="s">
+        <v>272</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I383" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix hydrogen supply input in hydrogen markets
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-distribution.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1AFB7F-A572-8442-9B68-EA4C5C5ADC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390F1383-229A-014D-8BE8-2BAB8D47B4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1600" windowWidth="27820" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="1600" windowWidth="25800" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1234,7 +1234,7 @@
   <dimension ref="A1:T364"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update wrt to 2.3.0.dev1
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-distribution.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1AFB7F-A572-8442-9B68-EA4C5C5ADC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390F1383-229A-014D-8BE8-2BAB8D47B4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1600" windowWidth="27820" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="1600" windowWidth="25800" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1234,7 +1234,7 @@
   <dimension ref="A1:T364"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>